<commit_message>
Hola mundo de pirobos
</commit_message>
<xml_diff>
--- a/Doo-Doc/Seccion # 6/Modelo de dominio anémico de contextos-VictusResidencias.xlsx
+++ b/Doo-Doc/Seccion # 6/Modelo de dominio anémico de contextos-VictusResidencias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Seccion # 6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3396E420-DA58-497B-AD70-AF84ADCA6AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{3396E420-DA58-497B-AD70-AF84ADCA6AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14BFE430-036A-45C0-BB3A-F2A94696FC0E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{082AFB46-52C9-4E4C-AE4E-19443AA1B53B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{082AFB46-52C9-4E4C-AE4E-19443AA1B53B}"/>
   </bookViews>
   <sheets>
     <sheet name="Valores" sheetId="3" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="Reservas" sheetId="6" r:id="rId6"/>
     <sheet name="Reserva-0001" sheetId="8" r:id="rId7"/>
     <sheet name="Reserva-0002" sheetId="9" r:id="rId8"/>
-    <sheet name="CaracterizaciónContexto1" sheetId="7" r:id="rId9"/>
+    <sheet name="Residente-0001" sheetId="10" r:id="rId9"/>
+    <sheet name="CaracterizaciónContexto1" sheetId="7" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="115">
   <si>
     <t>Problema/Dominio:</t>
   </si>
@@ -1113,6 +1114,30 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1138,30 +1163,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1607,20 +1608,20 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="26" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="2"/>
+    <col min="2" max="2" width="79.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="50" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="51"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
@@ -1636,7 +1637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="43.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="42" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>7</v>
       </c>
@@ -1644,43 +1645,43 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>22</v>
       </c>
@@ -1688,6 +1689,205 @@
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA574C3-CD54-44A7-8A00-D1CB8315B9A2}">
+  <dimension ref="A1:S5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" style="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="58" style="36" customWidth="1"/>
+    <col min="19" max="19" width="17.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="93">
+        <f>'[1]Configuración Apuestas'!D10</f>
+        <v>0</v>
+      </c>
+      <c r="C1" s="93"/>
+      <c r="D1" s="93"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="93"/>
+      <c r="R1" s="93"/>
+      <c r="S1" s="94"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="71"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="76" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77" t="s">
+        <v>66</v>
+      </c>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="78" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="80" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q4" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="R4" s="95"/>
+      <c r="S4" s="96"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="33"/>
+      <c r="K5" s="33"/>
+      <c r="L5" s="33"/>
+      <c r="M5" s="33"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="35"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="J3:Q3"/>
+    <mergeCell ref="R3:R4"/>
+    <mergeCell ref="S3:S4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1701,7 +1901,7 @@
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1716,15 +1916,15 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.7109375" style="7" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="36.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" style="7" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1734,7 +1934,7 @@
       <c r="C1" s="52"/>
       <c r="D1" s="53"/>
     </row>
-    <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -1744,7 +1944,7 @@
       <c r="C2" s="55"/>
       <c r="D2" s="56"/>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="57" t="s">
         <v>2</v>
       </c>
@@ -1752,7 +1952,7 @@
       <c r="C3" s="58"/>
       <c r="D3" s="59"/>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
@@ -1766,7 +1966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="61" t="s">
         <v>6</v>
       </c>
@@ -1780,7 +1980,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="61"/>
       <c r="B6" s="62"/>
       <c r="C6" s="37" t="s">
@@ -1788,7 +1988,7 @@
       </c>
       <c r="D6" s="62"/>
     </row>
-    <row r="7" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="61"/>
       <c r="B7" s="62"/>
       <c r="C7" s="37" t="s">
@@ -1796,7 +1996,7 @@
       </c>
       <c r="D7" s="62"/>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="60" t="s">
         <v>6</v>
       </c>
@@ -1810,7 +2010,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="60"/>
       <c r="B9" s="60"/>
       <c r="C9" s="38" t="s">
@@ -1818,7 +2018,7 @@
       </c>
       <c r="D9" s="60"/>
     </row>
-    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="60"/>
       <c r="B10" s="60"/>
       <c r="C10" s="38" t="s">
@@ -1826,7 +2026,7 @@
       </c>
       <c r="D10" s="60"/>
     </row>
-    <row r="11" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>6</v>
       </c>
@@ -1881,22 +2081,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{450F8E16-67C6-432D-A5AA-BF67F960EE18}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="64" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="18"/>
+    <col min="7" max="16384" width="11.44140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>38</v>
       </c>
@@ -1909,7 +2109,7 @@
       <c r="E1" s="63"/>
       <c r="F1" s="64"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>39</v>
       </c>
@@ -1922,7 +2122,7 @@
       <c r="E2" s="65"/>
       <c r="F2" s="66"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -1935,7 +2135,7 @@
       <c r="E3" s="67"/>
       <c r="F3" s="68"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="69" t="s">
         <v>40</v>
       </c>
@@ -1945,7 +2145,7 @@
       <c r="E4" s="70"/>
       <c r="F4" s="71"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>41</v>
       </c>
@@ -1963,7 +2163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>45</v>
       </c>
@@ -1975,7 +2175,7 @@
       <c r="E6" s="72"/>
       <c r="F6" s="73"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>47</v>
       </c>
@@ -1991,7 +2191,7 @@
       </c>
       <c r="F7" s="73"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>50</v>
       </c>
@@ -2012,7 +2212,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
         <v>25</v>
       </c>
@@ -2064,21 +2264,21 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="64" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="18"/>
+    <col min="7" max="16384" width="11.44140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>38</v>
       </c>
@@ -2091,7 +2291,7 @@
       <c r="E1" s="63"/>
       <c r="F1" s="64"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>39</v>
       </c>
@@ -2104,7 +2304,7 @@
       <c r="E2" s="65"/>
       <c r="F2" s="66"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -2117,7 +2317,7 @@
       <c r="E3" s="67"/>
       <c r="F3" s="68"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="69" t="s">
         <v>40</v>
       </c>
@@ -2127,7 +2327,7 @@
       <c r="E4" s="70"/>
       <c r="F4" s="71"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>41</v>
       </c>
@@ -2145,7 +2345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>45</v>
       </c>
@@ -2157,7 +2357,7 @@
       <c r="E6" s="72"/>
       <c r="F6" s="73"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>47</v>
       </c>
@@ -2173,7 +2373,7 @@
       </c>
       <c r="F7" s="73"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>30</v>
       </c>
@@ -2194,7 +2394,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
         <v>31</v>
       </c>
@@ -2245,22 +2445,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C088BE7-88A8-46E0-AF18-6F40B3F602F8}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.88671875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="64" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="11.42578125" style="18"/>
+    <col min="7" max="16384" width="11.44140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>38</v>
       </c>
@@ -2273,7 +2473,7 @@
       <c r="E1" s="63"/>
       <c r="F1" s="64"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>39</v>
       </c>
@@ -2286,7 +2486,7 @@
       <c r="E2" s="65"/>
       <c r="F2" s="66"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
@@ -2299,7 +2499,7 @@
       <c r="E3" s="67"/>
       <c r="F3" s="68"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="69" t="s">
         <v>40</v>
       </c>
@@ -2309,7 +2509,7 @@
       <c r="E4" s="70"/>
       <c r="F4" s="71"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>41</v>
       </c>
@@ -2327,7 +2527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="20" t="s">
         <v>45</v>
       </c>
@@ -2339,7 +2539,7 @@
       <c r="E6" s="72"/>
       <c r="F6" s="73"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="20" t="s">
         <v>47</v>
       </c>
@@ -2355,7 +2555,7 @@
       </c>
       <c r="F7" s="73"/>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="23" t="s">
         <v>29</v>
       </c>
@@ -2376,7 +2576,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="28" t="s">
         <v>59</v>
       </c>
@@ -2427,61 +2627,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3888799-E6A1-4FAB-A09B-AF9FE652AF52}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="58" style="36" customWidth="1"/>
-    <col min="19" max="19" width="17.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="18"/>
+    <col min="19" max="19" width="17.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="83" t="str">
+      <c r="B1" s="74" t="str">
         <f>Reservas!D8</f>
         <v>Reserva-0001</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="84"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="75"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
@@ -2502,36 +2702,36 @@
       <c r="R2" s="70"/>
       <c r="S2" s="71"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="85" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="87" t="s">
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="89" t="s">
+      <c r="S3" s="80" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
         <v>38</v>
       </c>
@@ -2583,14 +2783,14 @@
       <c r="Q4" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="R4" s="88"/>
-      <c r="S4" s="90"/>
-    </row>
-    <row r="5" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="74" t="s">
+      <c r="R4" s="79"/>
+      <c r="S4" s="81"/>
+    </row>
+    <row r="5" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="82" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="84" t="s">
         <v>81</v>
       </c>
       <c r="C5" s="42" t="s">
@@ -2629,13 +2829,13 @@
       <c r="R5" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="S5" s="80" t="s">
+      <c r="S5" s="88" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="74"/>
-      <c r="B6" s="76"/>
+    <row r="6" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="82"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="42" t="s">
         <v>83</v>
       </c>
@@ -2672,11 +2872,11 @@
       <c r="R6" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="S6" s="81"/>
-    </row>
-    <row r="7" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="74"/>
-      <c r="B7" s="76"/>
+      <c r="S6" s="89"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="82"/>
+      <c r="B7" s="84"/>
       <c r="C7" s="42" t="s">
         <v>88</v>
       </c>
@@ -2697,11 +2897,11 @@
       <c r="P7" s="42"/>
       <c r="Q7" s="42"/>
       <c r="R7" s="43"/>
-      <c r="S7" s="81"/>
-    </row>
-    <row r="8" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="74"/>
-      <c r="B8" s="77" t="s">
+      <c r="S7" s="89"/>
+    </row>
+    <row r="8" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="82"/>
+      <c r="B8" s="85" t="s">
         <v>88</v>
       </c>
       <c r="C8" s="44" t="s">
@@ -2740,11 +2940,11 @@
       <c r="R8" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="S8" s="81"/>
-    </row>
-    <row r="9" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="74"/>
-      <c r="B9" s="77"/>
+      <c r="S8" s="89"/>
+    </row>
+    <row r="9" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="82"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="44" t="s">
         <v>83</v>
       </c>
@@ -2781,11 +2981,11 @@
       <c r="R9" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="S9" s="81"/>
-    </row>
-    <row r="10" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
-      <c r="B10" s="77"/>
+      <c r="S9" s="89"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="82"/>
+      <c r="B10" s="85"/>
       <c r="C10" s="44" t="s">
         <v>89</v>
       </c>
@@ -2806,11 +3006,11 @@
       <c r="P10" s="44"/>
       <c r="Q10" s="44"/>
       <c r="R10" s="45"/>
-      <c r="S10" s="81"/>
-    </row>
-    <row r="11" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="74"/>
-      <c r="B11" s="78" t="s">
+      <c r="S10" s="89"/>
+    </row>
+    <row r="11" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="82"/>
+      <c r="B11" s="86" t="s">
         <v>89</v>
       </c>
       <c r="C11" s="46" t="s">
@@ -2849,11 +3049,11 @@
       <c r="R11" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="S11" s="81"/>
-    </row>
-    <row r="12" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="75"/>
-      <c r="B12" s="79"/>
+      <c r="S11" s="89"/>
+    </row>
+    <row r="12" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="83"/>
+      <c r="B12" s="87"/>
       <c r="C12" s="48" t="s">
         <v>83</v>
       </c>
@@ -2890,21 +3090,21 @@
       <c r="R12" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="S12" s="82"/>
+      <c r="S12" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="S5:S12"/>
     <mergeCell ref="B1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="J3:Q3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="S5:S12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2914,61 +3114,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC2EBB7-5669-4BC7-8C4D-6FF94FADDE33}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="77" workbookViewId="0">
       <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" style="18" customWidth="1"/>
     <col min="2" max="2" width="21" style="18" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" style="18" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.44140625" style="18" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="31" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="58" style="36" customWidth="1"/>
-    <col min="19" max="19" width="17.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="18"/>
+    <col min="19" max="19" width="17.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="83" t="str">
+      <c r="B1" s="74" t="str">
         <f>Reservas!D9</f>
         <v>Reserva-0002</v>
       </c>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
-      <c r="F1" s="83"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
-      <c r="I1" s="83"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="83"/>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="83"/>
-      <c r="O1" s="83"/>
-      <c r="P1" s="83"/>
-      <c r="Q1" s="83"/>
-      <c r="R1" s="83"/>
-      <c r="S1" s="84"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="75"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="69"/>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
@@ -2989,36 +3189,36 @@
       <c r="R2" s="70"/>
       <c r="S2" s="71"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="85" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="87" t="s">
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="89" t="s">
+      <c r="S3" s="80" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="40" t="s">
         <v>38</v>
       </c>
@@ -3070,14 +3270,14 @@
       <c r="Q4" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="R4" s="88"/>
-      <c r="S4" s="90"/>
-    </row>
-    <row r="5" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R4" s="79"/>
+      <c r="S4" s="81"/>
+    </row>
+    <row r="5" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="76" t="s">
+      <c r="B5" s="84" t="s">
         <v>99</v>
       </c>
       <c r="C5" s="42" t="s">
@@ -3116,13 +3316,13 @@
       <c r="R5" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="S5" s="80" t="s">
+      <c r="S5" s="88" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="91"/>
-      <c r="B6" s="76"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="42" t="s">
         <v>83</v>
       </c>
@@ -3159,11 +3359,11 @@
       <c r="R6" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="S6" s="81"/>
-    </row>
-    <row r="7" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S6" s="89"/>
+    </row>
+    <row r="7" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="91"/>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="85" t="s">
         <v>59</v>
       </c>
       <c r="C7" s="44" t="s">
@@ -3202,11 +3402,11 @@
       <c r="R7" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="S7" s="81"/>
-    </row>
-    <row r="8" spans="1:19" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S7" s="89"/>
+    </row>
+    <row r="8" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="91"/>
-      <c r="B8" s="77"/>
+      <c r="B8" s="85"/>
       <c r="C8" s="44" t="s">
         <v>83</v>
       </c>
@@ -3243,11 +3443,11 @@
       <c r="R8" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="S8" s="81"/>
-    </row>
-    <row r="9" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S8" s="89"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="91"/>
-      <c r="B9" s="77"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="44" t="s">
         <v>101</v>
       </c>
@@ -3268,11 +3468,11 @@
       <c r="P9" s="44"/>
       <c r="Q9" s="44"/>
       <c r="R9" s="45"/>
-      <c r="S9" s="81"/>
-    </row>
-    <row r="10" spans="1:19" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S9" s="89"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="91"/>
-      <c r="B10" s="77"/>
+      <c r="B10" s="85"/>
       <c r="C10" s="44" t="s">
         <v>102</v>
       </c>
@@ -3293,11 +3493,11 @@
       <c r="P10" s="44"/>
       <c r="Q10" s="44"/>
       <c r="R10" s="45"/>
-      <c r="S10" s="81"/>
-    </row>
-    <row r="11" spans="1:19" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S10" s="89"/>
+    </row>
+    <row r="11" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="91"/>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="86" t="s">
         <v>100</v>
       </c>
       <c r="C11" s="46" t="s">
@@ -3336,11 +3536,11 @@
       <c r="R11" s="47" t="s">
         <v>113</v>
       </c>
-      <c r="S11" s="81"/>
-    </row>
-    <row r="12" spans="1:19" ht="61.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S11" s="89"/>
+    </row>
+    <row r="12" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="92"/>
-      <c r="B12" s="79"/>
+      <c r="B12" s="87"/>
       <c r="C12" s="48" t="s">
         <v>83</v>
       </c>
@@ -3377,88 +3577,86 @@
       <c r="R12" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="S12" s="82"/>
+      <c r="S12" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="S5:S12"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="B1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="J3:Q3"/>
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="S3:S4"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="S5:S12"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA574C3-CD54-44A7-8A00-D1CB8315B9A2}">
-  <dimension ref="A1:S5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B91709D-862F-47AE-9690-135FDFD3E8F1}">
+  <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5703125" style="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.5703125" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.44140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5546875" style="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" style="18" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="58" style="36" customWidth="1"/>
-    <col min="19" max="19" width="17.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="18"/>
+    <col min="19" max="19" width="17.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="93">
-        <f>'[1]Configuración Apuestas'!D10</f>
-        <v>0</v>
-      </c>
-      <c r="C1" s="93"/>
-      <c r="D1" s="93"/>
-      <c r="E1" s="93"/>
-      <c r="F1" s="93"/>
-      <c r="G1" s="93"/>
-      <c r="H1" s="93"/>
-      <c r="I1" s="93"/>
-      <c r="J1" s="93"/>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="94"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
-        <v>64</v>
-      </c>
+      <c r="B1" s="74" t="str">
+        <f>Reservas!D8</f>
+        <v>Reserva-0001</v>
+      </c>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
+      <c r="P1" s="74"/>
+      <c r="Q1" s="74"/>
+      <c r="R1" s="74"/>
+      <c r="S1" s="75"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="69"/>
       <c r="B2" s="70"/>
       <c r="C2" s="70"/>
       <c r="D2" s="70"/>
@@ -3478,113 +3676,403 @@
       <c r="R2" s="70"/>
       <c r="S2" s="71"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="85" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86" t="s">
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="87" t="s">
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="77"/>
+      <c r="N3" s="77"/>
+      <c r="O3" s="77"/>
+      <c r="P3" s="77"/>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="89" t="s">
+      <c r="S3" s="80" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="21" t="s">
+      <c r="D4" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="G4" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="21" t="s">
+      <c r="H4" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="I4" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="K4" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="L4" s="21" t="s">
+      <c r="L4" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="M4" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="N4" s="21" t="s">
+      <c r="N4" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="O4" s="21" t="s">
+      <c r="O4" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="P4" s="21" t="s">
+      <c r="P4" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="Q4" s="21" t="s">
+      <c r="Q4" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="R4" s="95"/>
-      <c r="S4" s="96"/>
-    </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="35"/>
+      <c r="R4" s="79"/>
+      <c r="S4" s="81"/>
+    </row>
+    <row r="5" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="84" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="42">
+        <v>32</v>
+      </c>
+      <c r="F5" s="42">
+        <v>32</v>
+      </c>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5" s="42">
+        <v>32</v>
+      </c>
+      <c r="N5" s="42">
+        <v>32</v>
+      </c>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="42"/>
+      <c r="R5" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="S5" s="88" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="82"/>
+      <c r="B6" s="84"/>
+      <c r="C6" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="42">
+        <v>1</v>
+      </c>
+      <c r="F6" s="42">
+        <v>50</v>
+      </c>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="L6" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="M6" s="42">
+        <v>1</v>
+      </c>
+      <c r="N6" s="42">
+        <v>50</v>
+      </c>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="S6" s="89"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="82"/>
+      <c r="B7" s="84"/>
+      <c r="C7" s="42" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="42"/>
+      <c r="O7" s="42"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="89"/>
+    </row>
+    <row r="8" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="82"/>
+      <c r="B8" s="85" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="44">
+        <v>32</v>
+      </c>
+      <c r="F8" s="44">
+        <v>32</v>
+      </c>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44" t="s">
+        <v>90</v>
+      </c>
+      <c r="K8" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="L8" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="M8" s="44">
+        <v>32</v>
+      </c>
+      <c r="N8" s="44">
+        <v>32</v>
+      </c>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="S8" s="89"/>
+    </row>
+    <row r="9" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="82"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="44">
+        <v>1</v>
+      </c>
+      <c r="F9" s="44">
+        <v>50</v>
+      </c>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="L9" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" s="44">
+        <v>1</v>
+      </c>
+      <c r="N9" s="44">
+        <v>50</v>
+      </c>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="S9" s="89"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="82"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="44"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="44"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="89"/>
+    </row>
+    <row r="11" spans="1:19" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="82"/>
+      <c r="B11" s="86" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="46">
+        <v>32</v>
+      </c>
+      <c r="F11" s="46">
+        <v>32</v>
+      </c>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="K11" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="L11" s="46" t="s">
+        <v>80</v>
+      </c>
+      <c r="M11" s="46">
+        <v>32</v>
+      </c>
+      <c r="N11" s="46">
+        <v>32</v>
+      </c>
+      <c r="O11" s="46"/>
+      <c r="P11" s="46"/>
+      <c r="Q11" s="46"/>
+      <c r="R11" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="S11" s="89"/>
+    </row>
+    <row r="12" spans="1:19" ht="44.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="83"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="48">
+        <v>1</v>
+      </c>
+      <c r="F12" s="48">
+        <v>50</v>
+      </c>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="K12" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="L12" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="M12" s="48">
+        <v>1</v>
+      </c>
+      <c r="N12" s="48">
+        <v>50</v>
+      </c>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="S12" s="90"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="S5:S12"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B12"/>
     <mergeCell ref="B1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:I3"/>

</xml_diff>